<commit_message>
feat: add Excel helper functions for column operations, cell merging, and image insertion
- Implement toColumnName and toColumnIndex helpers for dynamic column calculations
- Add mergeCell helper to support cell range merging with auto-deduplication
- Implement img helper for inserting base64-encoded images into Excel files
  - Support PNG, JPEG, WebP, BMP, TIFF, GIF formats
  - Use oneCellAnchor mode to prevent image deformation
  - Generate UUID-based relationship IDs to avoid conflicts
  - Auto-generate drawing.xml, drawing.xml.rels, and sheet.xml.rels
  - Update [Content_Types].xml with drawing declarations
- Update documentation (README.md and README_CN.md) with detailed usage examples
</commit_message>
<xml_diff>
--- a/examples/template.xlsx
+++ b/examples/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hugjs\github\xlsx-handlebars\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D23420B-99B6-449F-950E-3559430CEA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D83264-4F2F-4228-B67C-2C3BFA795DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1660" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="1610" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>员工姓名:</t>
   </si>
@@ -111,88 +111,106 @@
     </r>
   </si>
   <si>
+    <t>{{name}}</t>
+  </si>
+  <si>
+    <t>{{status}}1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{status}}2{{/each}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖金:</t>
+  </si>
+  <si>
+    <r>
+      <t>{{removeRow}}{{#each proj</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF4EA72E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ects}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>¥{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employee.bonus_amount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FFEE0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{num employee.bonus_amount}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{formula "=SUM(A1:B1)"}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并单元格:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{formula (concat "=SUM(" (_c) "1:" (_c) "10)")}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>- {{name}}: {{description}} ({{status}}){{/each}}</t>
-  </si>
-  <si>
-    <t>{{name}}</t>
-  </si>
-  <si>
-    <t>{{status}}1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{status}}2{{/each}}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖金:</t>
-  </si>
-  <si>
-    <r>
-      <t>{{removeRow}}{{#each proj</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF4EA72E"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ects}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>¥{{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>employee.bonus_amount</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FFEE0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>}}</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{num employee.bonus_amount}}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{formula "=SUM(A1:B1)"}}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{formula (concat "=SUM(" (_c) "1:" (_c) "10)")}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{img image.base64}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{employee.name}}--{{mergeCell (concat "B" (_r) ":C" (_r))}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -275,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -285,6 +303,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -565,15 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -582,10 +601,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
       <c r="F1">
         <v>12</v>
@@ -624,37 +643,56 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="54" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleteCurrentSheet, setCurrentSheetName, hideCurrentSheet, hyperlink
</commit_message>
<xml_diff>
--- a/examples/template.xlsx
+++ b/examples/template.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hugjs\github\xlsx-handlebars\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D83264-4F2F-4228-B67C-2C3BFA795DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC3EFF2-8A8B-4667-B4CF-401472BA13E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1610" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="1030" windowWidth="19200" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="被删除的工作表" sheetId="2" r:id="rId2"/>
+    <sheet name="被隐藏的工作表" sheetId="3" r:id="rId3"/>
+    <sheet name="被链接的工作表" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>员工姓名:</t>
   </si>
@@ -212,12 +215,36 @@
     <t>{{employee.name}}--{{mergeCell (concat "B" (_r) ":C" (_r))}}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>{{deleteCurrentSheet}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作表命名:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{setCurrentSheetName "new sheet name"}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{hideCurrentSheet}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>静态合并单元格</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +299,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,10 +325,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -304,9 +340,14 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -596,7 +637,7 @@
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -609,8 +650,14 @@
       <c r="F1">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -626,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -634,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,17 +689,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -663,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -671,12 +718,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -693,10 +740,86 @@
       </c>
       <c r="D18" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A26" location="被链接的工作表!A1" display="链接" xr:uid="{15B58625-0F0E-400C-B9B4-3E6F2D4BF5CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64C8C7D-C11A-4BF5-A973-DEF6E625B760}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01CCD4A-9B7C-4E5C-BBAB-23E622E2F30C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4446C4-1CC5-4D21-9A0F-BDE531A64E55}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>